<commit_message>
feat: implement spreadsheet input, transformation, visualization, and testing
</commit_message>
<xml_diff>
--- a/planilha_convertida.xlsx
+++ b/planilha_convertida.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +609,51 @@
           <t>My-c10</t>
         </is>
       </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Fz-c11</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Mx-c11</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>My-c11</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Fz-c12</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Mx-c12</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>My-c12</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Fz-c13</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Mx-c13</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>My-c13</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -720,6 +765,33 @@
       <c r="AI2" t="n">
         <v>1</v>
       </c>
+      <c r="AJ2" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -831,6 +903,33 @@
       <c r="AI3" t="n">
         <v>1</v>
       </c>
+      <c r="AJ3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -942,6 +1041,33 @@
       <c r="AI4" t="n">
         <v>1</v>
       </c>
+      <c r="AJ4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1053,6 +1179,33 @@
       <c r="AI5" t="n">
         <v>1</v>
       </c>
+      <c r="AJ5" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1164,6 +1317,33 @@
       <c r="AI6" t="n">
         <v>1</v>
       </c>
+      <c r="AJ6" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1275,6 +1455,33 @@
       <c r="AI7" t="n">
         <v>1</v>
       </c>
+      <c r="AJ7" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1386,6 +1593,33 @@
       <c r="AI8" t="n">
         <v>1</v>
       </c>
+      <c r="AJ8" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1497,6 +1731,33 @@
       <c r="AI9" t="n">
         <v>1</v>
       </c>
+      <c r="AJ9" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1608,6 +1869,33 @@
       <c r="AI10" t="n">
         <v>1</v>
       </c>
+      <c r="AJ10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1718,6 +2006,33 @@
       </c>
       <c r="AI11" t="n">
         <v>1</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>26</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>